<commit_message>
Usuario, Carga Datos grabación
</commit_message>
<xml_diff>
--- a/Captura.xlsx
+++ b/Captura.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Proyectos\Ranorex\IQDOC_Sanitas\IQDOC_Sanitas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD666203-6D90-4EB9-80FB-FBE2079F0B8D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A709684-15D0-4F8E-8382-D7211A07EB14}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
+    <sheet name="Usuario" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$M$3</definedName>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14002" uniqueCount="2021">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14004" uniqueCount="2023">
   <si>
     <t>HC -- HONORARIO CONSULTORIO</t>
   </si>
@@ -6113,6 +6114,12 @@
   </si>
   <si>
     <t>555000</t>
+  </si>
+  <si>
+    <t>PruebasAuto60</t>
+  </si>
+  <si>
+    <t>Usuario</t>
   </si>
 </sst>
 </file>
@@ -6556,7 +6563,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView topLeftCell="H1" workbookViewId="0">
       <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
@@ -47629,7 +47636,7 @@
   <dimension ref="C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -55617,4 +55624,27 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC55A26B-90EE-4832-B935-97C01BE57916}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2021</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>